<commit_message>
Updated Mobile automation script of Transfer note
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Mobile-TransferNote.data.xlsx
+++ b/tests/artifact/data/Mobile-TransferNote.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="264">
   <si>
     <t>login.screen</t>
   </si>
@@ -184,7 +184,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>(//button[text()=' Open '])[106]</t>
+    <t>(//button[text()=' Open '])[1]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -616,13 +616,13 @@
     <t>SupplyDate</t>
   </si>
   <si>
-    <t>16-02-2024</t>
+    <t>22-02-2024</t>
   </si>
   <si>
     <t>receiptDate</t>
   </si>
   <si>
-    <t>20-02-2024</t>
+    <t>25-02-2024</t>
   </si>
   <si>
     <t>ctn.addItem</t>
@@ -821,6 +821,12 @@
   </si>
   <si>
     <t>//*[text()='Approve']</t>
+  </si>
+  <si>
+    <t>Mobile.data.xpath</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-body px-0']/div/div[2]/div/div/div[2]/table/tbody/tr[7]/td[2]div/input</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1945,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -3036,6 +3042,14 @@
         <v>261</v>
       </c>
     </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
UI Stock on Hand
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Mobile-TransferNote.data.xlsx
+++ b/tests/artifact/data/Mobile-TransferNote.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -30,30 +30,25 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="264">
-  <si>
-    <t>login.screen</t>
-  </si>
-  <si>
-    <t>//img[@alt='Banner']</t>
-  </si>
-  <si>
-    <t>login.screenheading</t>
-  </si>
-  <si>
-    <t>//*[@class='bottom_section__title']</t>
-  </si>
-  <si>
-    <t>login.logo</t>
-  </si>
-  <si>
-    <t>//*[@class='login__top_section']//*[name()='svg']</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="230">
   <si>
     <t>login.heading</t>
   </si>
@@ -61,78 +56,6 @@
     <t>//*[text() = 'Welcome to AccionConnect']</t>
   </si>
   <si>
-    <t>valid.username</t>
-  </si>
-  <si>
-    <t>crypt:21e9e83d0214461709b469d8e5e193ba1319ad9c4d4777da97d24a25737c11fe0b69b7a579e577d9</t>
-  </si>
-  <si>
-    <t>invalid.password</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>password.error</t>
-  </si>
-  <si>
-    <t>//div[@class ='OyEIQ uSvLId']</t>
-  </si>
-  <si>
-    <t>invalid.username</t>
-  </si>
-  <si>
-    <t>breeze@accionlabs.com</t>
-  </si>
-  <si>
-    <t>email.error</t>
-  </si>
-  <si>
-    <t>//div[@class='jXeDnc ']</t>
-  </si>
-  <si>
-    <t>AccountBoxIcon</t>
-  </si>
-  <si>
-    <t>(//span[@class='MuiTouchRipple-root css-w0pj6f'])[2]</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>//li[normalize-space(text())='Logout']</t>
-  </si>
-  <si>
-    <t>Login.logoutaccount</t>
-  </si>
-  <si>
-    <t>//*[@class = 'gb_e gb_0a gb_r']</t>
-  </si>
-  <si>
-    <t>Signout.url</t>
-  </si>
-  <si>
-    <t>https://accounts.google.com/Logout?hl=en&amp;continue=https://www.google.com/</t>
-  </si>
-  <si>
-    <t>Remove.account</t>
-  </si>
-  <si>
-    <t>(//div[@class='lCoei YZVTmd SmR8'])[3]</t>
-  </si>
-  <si>
-    <t>Remoe.button</t>
-  </si>
-  <si>
-    <t>//div/div[@class='n3x5Fb']</t>
-  </si>
-  <si>
-    <t>Remove.Yes.Account</t>
-  </si>
-  <si>
-    <t>(//span[@class='RveJvd snByac'])[3]</t>
-  </si>
-  <si>
     <t>login.clickDefault</t>
   </si>
   <si>
@@ -149,18 +72,6 @@
   </si>
   <si>
     <t>//input[@placeholder='Password']</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>crypt:64d8d2707c9e0cea4268fe56e98f05f63a6f8cf3bf5f75b9</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>crypt:ada9ee50d66e087dfe636dd530d88919199912d84dd3a9ed</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -832,14 +743,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -861,12 +772,6 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1354,152 +1259,152 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1523,11 +1428,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1589,13 +1490,27 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color theme="1"/>
+        <b val="0"/>
+        <i val="1"/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.349986266670736"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.249946592608417"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.599963377788629"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1615,25 +1530,25 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.249946592608417"/>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.599963377788629"/>
+          <bgColor theme="0" tint="-0.14996795556505"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b val="1"/>
         <i val="1"/>
         <strike val="0"/>
-        <color theme="0" tint="-0.349986266670736"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="2"/>
+          <bgColor theme="0" tint="-0.0499893185216834"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,20 +1563,6 @@
       <numFmt numFmtId="49" formatCode="@"/>
       <fill>
         <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="1"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.0499893185216834"/>
-        </patternFill>
       </fill>
     </dxf>
   </dxfs>
@@ -1945,10 +1846,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -1971,7 +1872,7 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2043,7 +1944,7 @@
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2091,7 +1992,7 @@
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2260,323 +2161,323 @@
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" ht="23.1" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="40" ht="23.1" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="41" ht="23.1" customHeight="1" spans="1:2">
       <c r="A41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
+    </row>
+    <row r="42" ht="23.1" customHeight="1" spans="1:3">
+      <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A45" s="4" t="s">
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A46" s="4" t="s">
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A49" s="4" t="s">
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A50" s="4" t="s">
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A51" s="4" t="s">
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A52" s="4" t="s">
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A53" s="4" t="s">
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A54" s="4" t="s">
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A55" s="4" t="s">
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A56" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A57" s="4" t="s">
         <v>111</v>
       </c>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A58" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B58" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" ht="23.1" customHeight="1" spans="1:3">
-      <c r="A59" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="8"/>
-    </row>
-    <row r="61" spans="1:3">
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="8"/>
-    </row>
-    <row r="62" spans="1:3">
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C62" s="8"/>
-    </row>
-    <row r="63" spans="1:3">
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="8"/>
-    </row>
-    <row r="64" spans="1:3">
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="8"/>
-    </row>
-    <row r="65" spans="1:3">
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C65" s="8"/>
-    </row>
-    <row r="66" spans="1:3">
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C66" s="8"/>
-    </row>
-    <row r="67" spans="1:3">
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="8"/>
-    </row>
-    <row r="68" spans="1:3">
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="8"/>
-    </row>
-    <row r="69" spans="1:3">
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C69" s="8"/>
-    </row>
-    <row r="70" spans="1:3">
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="8"/>
-    </row>
-    <row r="71" spans="1:3">
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C71" s="8"/>
-    </row>
-    <row r="72" spans="1:3">
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C72" s="8"/>
-    </row>
-    <row r="73" spans="1:3">
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C73" s="8"/>
-    </row>
-    <row r="74" spans="1:3">
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C74" s="8"/>
-    </row>
-    <row r="75" spans="1:3">
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="8"/>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
@@ -2751,481 +2652,315 @@
         <v>192</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="37" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="35" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A25,LEN("//"))="//"</formula>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="beginsWith" dxfId="0" priority="35" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A8,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="36" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A8,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="37" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A8,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="38" stopIfTrue="1">
+      <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="40">
-      <formula>LEN(TRIM(B25))&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="39" stopIfTrue="1">
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="4" priority="39" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="40">
+      <formula>LEN(TRIM(B8))&gt;0</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="53" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A26,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="54" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="55" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="56" stopIfTrue="1">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="beginsWith" dxfId="0" priority="53" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A9,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="54" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A9,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="55" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A9,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="56" stopIfTrue="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="57" stopIfTrue="1">
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="4" priority="57" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="58">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="58">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="3" priority="47" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="49" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="50" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="beginsWith" dxfId="0" priority="47" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A10,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="48" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A10,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="49" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A10,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="50" stopIfTrue="1">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="5" priority="51" stopIfTrue="1">
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="4" priority="51" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="52">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="52">
+      <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="beginsWith" dxfId="3" priority="41" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A28,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="43" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="44" stopIfTrue="1">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="beginsWith" dxfId="0" priority="41" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A11,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="42" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="43" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="44" stopIfTrue="1">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="5" priority="45" stopIfTrue="1">
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="4" priority="45" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
-      <formula>LEN(TRIM(B28))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="46">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A113">
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A113,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A113,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A113,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A113))&gt;0</formula>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A96,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A96,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A96,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="B96">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B113))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(B96))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="59" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A49:A50">
+    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A49,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A49,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A49,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(A49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A7 A12:A48 A51:A95 A97:A1048576">
+    <cfRule type="beginsWith" dxfId="0" priority="65" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="60" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="66" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="61" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="67" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="62" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="68" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66:A67">
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A66,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A66,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A66,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="63" stopIfTrue="1">
+  <conditionalFormatting sqref="C8:E42 B24:B42 B12:B22 B43:E95 C96:E96 B97:E1048576 B1:E7">
+    <cfRule type="expression" dxfId="4" priority="69" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="64">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="72">
       <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B21">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="26">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="25" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E59 B41:B59 B29:B39 B60:E112 C113:E113 B114:E1048576">
-    <cfRule type="expression" dxfId="5" priority="69" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="72">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A65 A68:A112 A114:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="65" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A4,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="66" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="67" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="68" stopIfTrue="1">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>